<commit_message>
Updating for version 20.4.1
</commit_message>
<xml_diff>
--- a/devnet_sbx_testbed.xlsx
+++ b/devnet_sbx_testbed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/claudia/Dropbox (Indigo Wire Networks)/scripts/python/2020/pyats_intro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1737A2BF-CBF3-C74A-BFB9-3188A5FF5ABC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDB58EA-76B5-4649-86DA-F56E2D8C48FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20520" yWindow="9440" windowWidth="28040" windowHeight="17440" xr2:uid="{B1CD2092-96F8-D541-AB83-A29EF0B7CE1F}"/>
+    <workbookView xWindow="9440" yWindow="9280" windowWidth="28040" windowHeight="17440" xr2:uid="{B1CD2092-96F8-D541-AB83-A29EF0B7CE1F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,9 +74,6 @@
     <t>nxos</t>
   </si>
   <si>
-    <t>iosze</t>
-  </si>
-  <si>
     <t>admin</t>
   </si>
   <si>
@@ -87,6 +84,9 @@
   </si>
   <si>
     <t>C1sco12345</t>
+  </si>
+  <si>
+    <t>iosxe</t>
   </si>
 </sst>
 </file>
@@ -441,7 +441,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,10 +480,10 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -503,10 +503,10 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -515,7 +515,7 @@
         <v>8181</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>